<commit_message>
Correcciones realizadas que impedian ejecutar el programa
</commit_message>
<xml_diff>
--- a/clustersEmpleados.xlsx
+++ b/clustersEmpleados.xlsx
@@ -622,7 +622,7 @@
         <v>1</v>
       </c>
       <c r="K5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -727,7 +727,7 @@
         <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -797,7 +797,7 @@
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
@@ -832,7 +832,7 @@
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
@@ -902,7 +902,7 @@
         <v>0</v>
       </c>
       <c r="K13" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14">
@@ -972,7 +972,7 @@
         <v>0</v>
       </c>
       <c r="K15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -1007,7 +1007,7 @@
         <v>0</v>
       </c>
       <c r="K16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -1147,7 +1147,7 @@
         <v>1</v>
       </c>
       <c r="K20" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1252,7 +1252,7 @@
         <v>0</v>
       </c>
       <c r="K23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
@@ -1322,7 +1322,7 @@
         <v>0</v>
       </c>
       <c r="K25" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26">
@@ -1357,7 +1357,7 @@
         <v>0</v>
       </c>
       <c r="K26" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27">
@@ -1427,7 +1427,7 @@
         <v>0</v>
       </c>
       <c r="K28" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29">
@@ -1497,7 +1497,7 @@
         <v>0</v>
       </c>
       <c r="K30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
@@ -1532,7 +1532,7 @@
         <v>0</v>
       </c>
       <c r="K31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -1672,7 +1672,7 @@
         <v>1</v>
       </c>
       <c r="K35" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -1777,7 +1777,7 @@
         <v>0</v>
       </c>
       <c r="K38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
@@ -1847,7 +1847,7 @@
         <v>0</v>
       </c>
       <c r="K40" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41">
@@ -1882,7 +1882,7 @@
         <v>0</v>
       </c>
       <c r="K41" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42">
@@ -1952,7 +1952,7 @@
         <v>0</v>
       </c>
       <c r="K43" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44">
@@ -2022,7 +2022,7 @@
         <v>0</v>
       </c>
       <c r="K45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46">
@@ -2057,7 +2057,7 @@
         <v>0</v>
       </c>
       <c r="K46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
@@ -2197,7 +2197,7 @@
         <v>1</v>
       </c>
       <c r="K50" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -2302,7 +2302,7 @@
         <v>0</v>
       </c>
       <c r="K53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54">
@@ -2372,7 +2372,7 @@
         <v>0</v>
       </c>
       <c r="K55" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56">
@@ -2407,7 +2407,7 @@
         <v>0</v>
       </c>
       <c r="K56" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57">
@@ -2477,7 +2477,7 @@
         <v>0</v>
       </c>
       <c r="K58" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59">
@@ -2547,7 +2547,7 @@
         <v>0</v>
       </c>
       <c r="K60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
@@ -2582,7 +2582,7 @@
         <v>0</v>
       </c>
       <c r="K61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62">
@@ -2722,7 +2722,7 @@
         <v>1</v>
       </c>
       <c r="K65" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -2827,7 +2827,7 @@
         <v>0</v>
       </c>
       <c r="K68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69">
@@ -2897,7 +2897,7 @@
         <v>0</v>
       </c>
       <c r="K70" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71">
@@ -2932,7 +2932,7 @@
         <v>0</v>
       </c>
       <c r="K71" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72">
@@ -3002,7 +3002,7 @@
         <v>0</v>
       </c>
       <c r="K73" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="74">
@@ -3072,7 +3072,7 @@
         <v>0</v>
       </c>
       <c r="K75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76">
@@ -3107,7 +3107,7 @@
         <v>0</v>
       </c>
       <c r="K76" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77">
@@ -3247,7 +3247,7 @@
         <v>1</v>
       </c>
       <c r="K80" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -3352,7 +3352,7 @@
         <v>0</v>
       </c>
       <c r="K83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84">
@@ -3422,7 +3422,7 @@
         <v>0</v>
       </c>
       <c r="K85" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="86">
@@ -3457,7 +3457,7 @@
         <v>0</v>
       </c>
       <c r="K86" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87">
@@ -3527,7 +3527,7 @@
         <v>0</v>
       </c>
       <c r="K88" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="89">
@@ -3597,7 +3597,7 @@
         <v>0</v>
       </c>
       <c r="K90" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91">
@@ -3632,7 +3632,7 @@
         <v>0</v>
       </c>
       <c r="K91" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92">
@@ -3772,7 +3772,7 @@
         <v>1</v>
       </c>
       <c r="K95" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96">
@@ -3877,7 +3877,7 @@
         <v>0</v>
       </c>
       <c r="K98" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99">
@@ -3947,7 +3947,7 @@
         <v>0</v>
       </c>
       <c r="K100" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="101">
@@ -3982,7 +3982,7 @@
         <v>0</v>
       </c>
       <c r="K101" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="102">
@@ -4052,7 +4052,7 @@
         <v>0</v>
       </c>
       <c r="K103" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="104">
@@ -4122,7 +4122,7 @@
         <v>0</v>
       </c>
       <c r="K105" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106">
@@ -4157,7 +4157,7 @@
         <v>0</v>
       </c>
       <c r="K106" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107">
@@ -4297,7 +4297,7 @@
         <v>1</v>
       </c>
       <c r="K110" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111">
@@ -4402,7 +4402,7 @@
         <v>0</v>
       </c>
       <c r="K113" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114">
@@ -4472,7 +4472,7 @@
         <v>0</v>
       </c>
       <c r="K115" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="116">
@@ -4507,7 +4507,7 @@
         <v>0</v>
       </c>
       <c r="K116" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="117">
@@ -4577,7 +4577,7 @@
         <v>0</v>
       </c>
       <c r="K118" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="119">
@@ -4647,7 +4647,7 @@
         <v>0</v>
       </c>
       <c r="K120" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121">
@@ -4682,7 +4682,7 @@
         <v>0</v>
       </c>
       <c r="K121" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122">
@@ -4822,7 +4822,7 @@
         <v>1</v>
       </c>
       <c r="K125" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126">
@@ -4927,7 +4927,7 @@
         <v>0</v>
       </c>
       <c r="K128" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129">
@@ -4997,7 +4997,7 @@
         <v>0</v>
       </c>
       <c r="K130" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="131">
@@ -5032,7 +5032,7 @@
         <v>0</v>
       </c>
       <c r="K131" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="132">
@@ -5102,7 +5102,7 @@
         <v>0</v>
       </c>
       <c r="K133" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="134">
@@ -5172,7 +5172,7 @@
         <v>0</v>
       </c>
       <c r="K135" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136">
@@ -5207,7 +5207,7 @@
         <v>0</v>
       </c>
       <c r="K136" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137">
@@ -5347,7 +5347,7 @@
         <v>1</v>
       </c>
       <c r="K140" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141">
@@ -5452,7 +5452,7 @@
         <v>0</v>
       </c>
       <c r="K143" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144">
@@ -5522,7 +5522,7 @@
         <v>0</v>
       </c>
       <c r="K145" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="146">
@@ -5557,7 +5557,7 @@
         <v>0</v>
       </c>
       <c r="K146" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="147">
@@ -5627,7 +5627,7 @@
         <v>0</v>
       </c>
       <c r="K148" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="149">
@@ -5697,7 +5697,7 @@
         <v>0</v>
       </c>
       <c r="K150" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151">
@@ -5732,7 +5732,7 @@
         <v>0</v>
       </c>
       <c r="K151" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152">
@@ -5872,7 +5872,7 @@
         <v>1</v>
       </c>
       <c r="K155" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="156">
@@ -5977,7 +5977,7 @@
         <v>0</v>
       </c>
       <c r="K158" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159">
@@ -6047,7 +6047,7 @@
         <v>0</v>
       </c>
       <c r="K160" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="161">
@@ -6082,7 +6082,7 @@
         <v>0</v>
       </c>
       <c r="K161" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="162">
@@ -6152,7 +6152,7 @@
         <v>0</v>
       </c>
       <c r="K163" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="164">
@@ -6222,7 +6222,7 @@
         <v>0</v>
       </c>
       <c r="K165" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="166">
@@ -6257,7 +6257,7 @@
         <v>0</v>
       </c>
       <c r="K166" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="167">
@@ -6397,7 +6397,7 @@
         <v>1</v>
       </c>
       <c r="K170" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="171">
@@ -6502,7 +6502,7 @@
         <v>0</v>
       </c>
       <c r="K173" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="174">
@@ -6572,7 +6572,7 @@
         <v>0</v>
       </c>
       <c r="K175" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="176">
@@ -6607,7 +6607,7 @@
         <v>0</v>
       </c>
       <c r="K176" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="177">
@@ -6677,7 +6677,7 @@
         <v>0</v>
       </c>
       <c r="K178" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="179">
@@ -6747,7 +6747,7 @@
         <v>0</v>
       </c>
       <c r="K180" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="181">
@@ -6782,7 +6782,7 @@
         <v>0</v>
       </c>
       <c r="K181" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="182">
@@ -6922,7 +6922,7 @@
         <v>1</v>
       </c>
       <c r="K185" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="186">
@@ -7027,7 +7027,7 @@
         <v>0</v>
       </c>
       <c r="K188" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="189">
@@ -7097,7 +7097,7 @@
         <v>0</v>
       </c>
       <c r="K190" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="191">
@@ -7132,7 +7132,7 @@
         <v>0</v>
       </c>
       <c r="K191" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="192">
@@ -7202,7 +7202,7 @@
         <v>0</v>
       </c>
       <c r="K193" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="194">
@@ -7272,7 +7272,7 @@
         <v>0</v>
       </c>
       <c r="K195" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="196">
@@ -7307,7 +7307,7 @@
         <v>0</v>
       </c>
       <c r="K196" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="197">
@@ -7447,7 +7447,7 @@
         <v>1</v>
       </c>
       <c r="K200" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="201">
@@ -7552,7 +7552,7 @@
         <v>0</v>
       </c>
       <c r="K203" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="204">
@@ -7622,7 +7622,7 @@
         <v>0</v>
       </c>
       <c r="K205" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="206">
@@ -7657,7 +7657,7 @@
         <v>0</v>
       </c>
       <c r="K206" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="207">
@@ -7727,7 +7727,7 @@
         <v>0</v>
       </c>
       <c r="K208" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="209">
@@ -7797,7 +7797,7 @@
         <v>0</v>
       </c>
       <c r="K210" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="211">
@@ -7832,7 +7832,7 @@
         <v>0</v>
       </c>
       <c r="K211" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="212">
@@ -7972,7 +7972,7 @@
         <v>1</v>
       </c>
       <c r="K215" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="216">
@@ -8077,7 +8077,7 @@
         <v>0</v>
       </c>
       <c r="K218" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="219">
@@ -8147,7 +8147,7 @@
         <v>0</v>
       </c>
       <c r="K220" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="221">
@@ -8182,7 +8182,7 @@
         <v>0</v>
       </c>
       <c r="K221" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="222">
@@ -8252,7 +8252,7 @@
         <v>0</v>
       </c>
       <c r="K223" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="224">
@@ -8322,7 +8322,7 @@
         <v>0</v>
       </c>
       <c r="K225" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="226">
@@ -8357,7 +8357,7 @@
         <v>0</v>
       </c>
       <c r="K226" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="227">
@@ -8497,7 +8497,7 @@
         <v>1</v>
       </c>
       <c r="K230" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="231">
@@ -8602,7 +8602,7 @@
         <v>0</v>
       </c>
       <c r="K233" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="234">
@@ -8672,7 +8672,7 @@
         <v>0</v>
       </c>
       <c r="K235" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="236">
@@ -8707,7 +8707,7 @@
         <v>0</v>
       </c>
       <c r="K236" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="237">
@@ -8777,7 +8777,7 @@
         <v>0</v>
       </c>
       <c r="K238" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="239">
@@ -8847,7 +8847,7 @@
         <v>0</v>
       </c>
       <c r="K240" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="241">
@@ -8882,7 +8882,7 @@
         <v>0</v>
       </c>
       <c r="K241" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="242">
@@ -9022,7 +9022,7 @@
         <v>1</v>
       </c>
       <c r="K245" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="246">
@@ -9127,7 +9127,7 @@
         <v>0</v>
       </c>
       <c r="K248" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="249">
@@ -9197,7 +9197,7 @@
         <v>0</v>
       </c>
       <c r="K250" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="251">
@@ -9232,7 +9232,7 @@
         <v>0</v>
       </c>
       <c r="K251" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="252">
@@ -9302,7 +9302,7 @@
         <v>0</v>
       </c>
       <c r="K253" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="254">
@@ -9372,7 +9372,7 @@
         <v>0</v>
       </c>
       <c r="K255" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="256">
@@ -9407,7 +9407,7 @@
         <v>0</v>
       </c>
       <c r="K256" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="257">
@@ -9547,7 +9547,7 @@
         <v>1</v>
       </c>
       <c r="K260" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="261">
@@ -9652,7 +9652,7 @@
         <v>0</v>
       </c>
       <c r="K263" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="264">
@@ -9722,7 +9722,7 @@
         <v>0</v>
       </c>
       <c r="K265" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="266">
@@ -9757,7 +9757,7 @@
         <v>0</v>
       </c>
       <c r="K266" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="267">
@@ -9827,7 +9827,7 @@
         <v>0</v>
       </c>
       <c r="K268" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="269">
@@ -9897,7 +9897,7 @@
         <v>0</v>
       </c>
       <c r="K270" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="271">
@@ -9932,7 +9932,7 @@
         <v>0</v>
       </c>
       <c r="K271" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Navegación de ventana principal a ventana perfilamiento
</commit_message>
<xml_diff>
--- a/clustersEmpleados.xlsx
+++ b/clustersEmpleados.xlsx
@@ -517,7 +517,7 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -587,7 +587,7 @@
         <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -622,7 +622,7 @@
         <v>1</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
@@ -657,7 +657,7 @@
         <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -727,7 +727,7 @@
         <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -797,7 +797,7 @@
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -832,7 +832,7 @@
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -867,7 +867,7 @@
         <v>1</v>
       </c>
       <c r="K12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13">
@@ -902,7 +902,7 @@
         <v>0</v>
       </c>
       <c r="K13" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -937,7 +937,7 @@
         <v>1</v>
       </c>
       <c r="K14" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15">
@@ -972,7 +972,7 @@
         <v>0</v>
       </c>
       <c r="K15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -1007,7 +1007,7 @@
         <v>0</v>
       </c>
       <c r="K16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -1042,7 +1042,7 @@
         <v>0</v>
       </c>
       <c r="K17" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18">
@@ -1112,7 +1112,7 @@
         <v>0</v>
       </c>
       <c r="K19" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -1147,7 +1147,7 @@
         <v>1</v>
       </c>
       <c r="K20" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21">
@@ -1182,7 +1182,7 @@
         <v>0</v>
       </c>
       <c r="K21" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -1252,7 +1252,7 @@
         <v>0</v>
       </c>
       <c r="K23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1322,7 +1322,7 @@
         <v>0</v>
       </c>
       <c r="K25" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -1357,7 +1357,7 @@
         <v>0</v>
       </c>
       <c r="K26" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -1392,7 +1392,7 @@
         <v>1</v>
       </c>
       <c r="K27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28">
@@ -1427,7 +1427,7 @@
         <v>0</v>
       </c>
       <c r="K28" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
@@ -1462,7 +1462,7 @@
         <v>1</v>
       </c>
       <c r="K29" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30">
@@ -1497,7 +1497,7 @@
         <v>0</v>
       </c>
       <c r="K30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -1532,7 +1532,7 @@
         <v>0</v>
       </c>
       <c r="K31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -1567,7 +1567,7 @@
         <v>0</v>
       </c>
       <c r="K32" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33">
@@ -1637,7 +1637,7 @@
         <v>0</v>
       </c>
       <c r="K34" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
@@ -1672,7 +1672,7 @@
         <v>1</v>
       </c>
       <c r="K35" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36">
@@ -1707,7 +1707,7 @@
         <v>0</v>
       </c>
       <c r="K36" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
@@ -1777,7 +1777,7 @@
         <v>0</v>
       </c>
       <c r="K38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -1847,7 +1847,7 @@
         <v>0</v>
       </c>
       <c r="K40" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
@@ -1882,7 +1882,7 @@
         <v>0</v>
       </c>
       <c r="K41" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -1917,7 +1917,7 @@
         <v>1</v>
       </c>
       <c r="K42" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43">
@@ -1952,7 +1952,7 @@
         <v>0</v>
       </c>
       <c r="K43" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44">
@@ -1987,7 +1987,7 @@
         <v>1</v>
       </c>
       <c r="K44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45">
@@ -2022,7 +2022,7 @@
         <v>0</v>
       </c>
       <c r="K45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -2057,7 +2057,7 @@
         <v>0</v>
       </c>
       <c r="K46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -2092,7 +2092,7 @@
         <v>0</v>
       </c>
       <c r="K47" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48">
@@ -2162,7 +2162,7 @@
         <v>0</v>
       </c>
       <c r="K49" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50">
@@ -2197,7 +2197,7 @@
         <v>1</v>
       </c>
       <c r="K50" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51">
@@ -2232,7 +2232,7 @@
         <v>0</v>
       </c>
       <c r="K51" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52">
@@ -2302,7 +2302,7 @@
         <v>0</v>
       </c>
       <c r="K53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -2372,7 +2372,7 @@
         <v>0</v>
       </c>
       <c r="K55" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56">
@@ -2407,7 +2407,7 @@
         <v>0</v>
       </c>
       <c r="K56" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57">
@@ -2442,7 +2442,7 @@
         <v>1</v>
       </c>
       <c r="K57" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58">
@@ -2477,7 +2477,7 @@
         <v>0</v>
       </c>
       <c r="K58" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59">
@@ -2512,7 +2512,7 @@
         <v>1</v>
       </c>
       <c r="K59" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60">
@@ -2547,7 +2547,7 @@
         <v>0</v>
       </c>
       <c r="K60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -2582,7 +2582,7 @@
         <v>0</v>
       </c>
       <c r="K61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -2617,7 +2617,7 @@
         <v>0</v>
       </c>
       <c r="K62" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63">
@@ -2687,7 +2687,7 @@
         <v>0</v>
       </c>
       <c r="K64" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65">
@@ -2722,7 +2722,7 @@
         <v>1</v>
       </c>
       <c r="K65" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66">
@@ -2757,7 +2757,7 @@
         <v>0</v>
       </c>
       <c r="K66" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67">
@@ -2827,7 +2827,7 @@
         <v>0</v>
       </c>
       <c r="K68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -2897,7 +2897,7 @@
         <v>0</v>
       </c>
       <c r="K70" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71">
@@ -2932,7 +2932,7 @@
         <v>0</v>
       </c>
       <c r="K71" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72">
@@ -2967,7 +2967,7 @@
         <v>1</v>
       </c>
       <c r="K72" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="73">
@@ -3002,7 +3002,7 @@
         <v>0</v>
       </c>
       <c r="K73" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74">
@@ -3037,7 +3037,7 @@
         <v>1</v>
       </c>
       <c r="K74" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75">
@@ -3072,7 +3072,7 @@
         <v>0</v>
       </c>
       <c r="K75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -3107,7 +3107,7 @@
         <v>0</v>
       </c>
       <c r="K76" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -3142,7 +3142,7 @@
         <v>0</v>
       </c>
       <c r="K77" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="78">
@@ -3212,7 +3212,7 @@
         <v>0</v>
       </c>
       <c r="K79" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80">
@@ -3247,7 +3247,7 @@
         <v>1</v>
       </c>
       <c r="K80" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81">
@@ -3282,7 +3282,7 @@
         <v>0</v>
       </c>
       <c r="K81" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82">
@@ -3352,7 +3352,7 @@
         <v>0</v>
       </c>
       <c r="K83" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84">
@@ -3422,7 +3422,7 @@
         <v>0</v>
       </c>
       <c r="K85" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86">
@@ -3457,7 +3457,7 @@
         <v>0</v>
       </c>
       <c r="K86" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87">
@@ -3492,7 +3492,7 @@
         <v>1</v>
       </c>
       <c r="K87" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="88">
@@ -3527,7 +3527,7 @@
         <v>0</v>
       </c>
       <c r="K88" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89">
@@ -3562,7 +3562,7 @@
         <v>1</v>
       </c>
       <c r="K89" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="90">
@@ -3597,7 +3597,7 @@
         <v>0</v>
       </c>
       <c r="K90" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91">
@@ -3632,7 +3632,7 @@
         <v>0</v>
       </c>
       <c r="K91" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92">
@@ -3667,7 +3667,7 @@
         <v>0</v>
       </c>
       <c r="K92" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="93">
@@ -3737,7 +3737,7 @@
         <v>0</v>
       </c>
       <c r="K94" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95">
@@ -3772,7 +3772,7 @@
         <v>1</v>
       </c>
       <c r="K95" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="96">
@@ -3807,7 +3807,7 @@
         <v>0</v>
       </c>
       <c r="K96" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97">
@@ -3877,7 +3877,7 @@
         <v>0</v>
       </c>
       <c r="K98" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99">
@@ -3947,7 +3947,7 @@
         <v>0</v>
       </c>
       <c r="K100" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101">
@@ -3982,7 +3982,7 @@
         <v>0</v>
       </c>
       <c r="K101" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102">
@@ -4017,7 +4017,7 @@
         <v>1</v>
       </c>
       <c r="K102" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="103">
@@ -4052,7 +4052,7 @@
         <v>0</v>
       </c>
       <c r="K103" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104">
@@ -4087,7 +4087,7 @@
         <v>1</v>
       </c>
       <c r="K104" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="105">
@@ -4122,7 +4122,7 @@
         <v>0</v>
       </c>
       <c r="K105" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106">
@@ -4157,7 +4157,7 @@
         <v>0</v>
       </c>
       <c r="K106" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107">
@@ -4192,7 +4192,7 @@
         <v>0</v>
       </c>
       <c r="K107" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="108">
@@ -4262,7 +4262,7 @@
         <v>0</v>
       </c>
       <c r="K109" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110">
@@ -4297,7 +4297,7 @@
         <v>1</v>
       </c>
       <c r="K110" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="111">
@@ -4332,7 +4332,7 @@
         <v>0</v>
       </c>
       <c r="K111" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112">
@@ -4402,7 +4402,7 @@
         <v>0</v>
       </c>
       <c r="K113" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114">
@@ -4472,7 +4472,7 @@
         <v>0</v>
       </c>
       <c r="K115" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116">
@@ -4507,7 +4507,7 @@
         <v>0</v>
       </c>
       <c r="K116" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117">
@@ -4542,7 +4542,7 @@
         <v>1</v>
       </c>
       <c r="K117" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="118">
@@ -4577,7 +4577,7 @@
         <v>0</v>
       </c>
       <c r="K118" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119">
@@ -4612,7 +4612,7 @@
         <v>1</v>
       </c>
       <c r="K119" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="120">
@@ -4647,7 +4647,7 @@
         <v>0</v>
       </c>
       <c r="K120" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121">
@@ -4682,7 +4682,7 @@
         <v>0</v>
       </c>
       <c r="K121" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122">
@@ -4717,7 +4717,7 @@
         <v>0</v>
       </c>
       <c r="K122" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="123">
@@ -4787,7 +4787,7 @@
         <v>0</v>
       </c>
       <c r="K124" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125">
@@ -4822,7 +4822,7 @@
         <v>1</v>
       </c>
       <c r="K125" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="126">
@@ -4857,7 +4857,7 @@
         <v>0</v>
       </c>
       <c r="K126" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127">
@@ -4927,7 +4927,7 @@
         <v>0</v>
       </c>
       <c r="K128" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129">
@@ -4997,7 +4997,7 @@
         <v>0</v>
       </c>
       <c r="K130" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131">
@@ -5032,7 +5032,7 @@
         <v>0</v>
       </c>
       <c r="K131" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132">
@@ -5067,7 +5067,7 @@
         <v>1</v>
       </c>
       <c r="K132" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="133">
@@ -5102,7 +5102,7 @@
         <v>0</v>
       </c>
       <c r="K133" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134">
@@ -5137,7 +5137,7 @@
         <v>1</v>
       </c>
       <c r="K134" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="135">
@@ -5172,7 +5172,7 @@
         <v>0</v>
       </c>
       <c r="K135" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136">
@@ -5207,7 +5207,7 @@
         <v>0</v>
       </c>
       <c r="K136" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137">
@@ -5242,7 +5242,7 @@
         <v>0</v>
       </c>
       <c r="K137" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="138">
@@ -5312,7 +5312,7 @@
         <v>0</v>
       </c>
       <c r="K139" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140">
@@ -5347,7 +5347,7 @@
         <v>1</v>
       </c>
       <c r="K140" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="141">
@@ -5382,7 +5382,7 @@
         <v>0</v>
       </c>
       <c r="K141" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142">
@@ -5452,7 +5452,7 @@
         <v>0</v>
       </c>
       <c r="K143" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144">
@@ -5522,7 +5522,7 @@
         <v>0</v>
       </c>
       <c r="K145" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146">
@@ -5557,7 +5557,7 @@
         <v>0</v>
       </c>
       <c r="K146" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147">
@@ -5592,7 +5592,7 @@
         <v>1</v>
       </c>
       <c r="K147" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="148">
@@ -5627,7 +5627,7 @@
         <v>0</v>
       </c>
       <c r="K148" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149">
@@ -5662,7 +5662,7 @@
         <v>1</v>
       </c>
       <c r="K149" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="150">
@@ -5697,7 +5697,7 @@
         <v>0</v>
       </c>
       <c r="K150" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151">
@@ -5732,7 +5732,7 @@
         <v>0</v>
       </c>
       <c r="K151" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152">
@@ -5767,7 +5767,7 @@
         <v>0</v>
       </c>
       <c r="K152" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="153">
@@ -5837,7 +5837,7 @@
         <v>0</v>
       </c>
       <c r="K154" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155">
@@ -5872,7 +5872,7 @@
         <v>1</v>
       </c>
       <c r="K155" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="156">
@@ -5907,7 +5907,7 @@
         <v>0</v>
       </c>
       <c r="K156" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157">
@@ -5977,7 +5977,7 @@
         <v>0</v>
       </c>
       <c r="K158" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="159">
@@ -6047,7 +6047,7 @@
         <v>0</v>
       </c>
       <c r="K160" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161">
@@ -6082,7 +6082,7 @@
         <v>0</v>
       </c>
       <c r="K161" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="162">
@@ -6117,7 +6117,7 @@
         <v>1</v>
       </c>
       <c r="K162" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="163">
@@ -6152,7 +6152,7 @@
         <v>0</v>
       </c>
       <c r="K163" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164">
@@ -6187,7 +6187,7 @@
         <v>1</v>
       </c>
       <c r="K164" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="165">
@@ -6222,7 +6222,7 @@
         <v>0</v>
       </c>
       <c r="K165" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="166">
@@ -6257,7 +6257,7 @@
         <v>0</v>
       </c>
       <c r="K166" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="167">
@@ -6292,7 +6292,7 @@
         <v>0</v>
       </c>
       <c r="K167" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="168">
@@ -6362,7 +6362,7 @@
         <v>0</v>
       </c>
       <c r="K169" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="170">
@@ -6397,7 +6397,7 @@
         <v>1</v>
       </c>
       <c r="K170" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="171">
@@ -6432,7 +6432,7 @@
         <v>0</v>
       </c>
       <c r="K171" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="172">
@@ -6502,7 +6502,7 @@
         <v>0</v>
       </c>
       <c r="K173" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="174">
@@ -6572,7 +6572,7 @@
         <v>0</v>
       </c>
       <c r="K175" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="176">
@@ -6607,7 +6607,7 @@
         <v>0</v>
       </c>
       <c r="K176" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177">
@@ -6642,7 +6642,7 @@
         <v>1</v>
       </c>
       <c r="K177" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="178">
@@ -6677,7 +6677,7 @@
         <v>0</v>
       </c>
       <c r="K178" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="179">
@@ -6712,7 +6712,7 @@
         <v>1</v>
       </c>
       <c r="K179" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="180">
@@ -6747,7 +6747,7 @@
         <v>0</v>
       </c>
       <c r="K180" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="181">
@@ -6782,7 +6782,7 @@
         <v>0</v>
       </c>
       <c r="K181" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="182">
@@ -6817,7 +6817,7 @@
         <v>0</v>
       </c>
       <c r="K182" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="183">
@@ -6887,7 +6887,7 @@
         <v>0</v>
       </c>
       <c r="K184" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="185">
@@ -6922,7 +6922,7 @@
         <v>1</v>
       </c>
       <c r="K185" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="186">
@@ -6957,7 +6957,7 @@
         <v>0</v>
       </c>
       <c r="K186" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="187">
@@ -7027,7 +7027,7 @@
         <v>0</v>
       </c>
       <c r="K188" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="189">
@@ -7097,7 +7097,7 @@
         <v>0</v>
       </c>
       <c r="K190" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="191">
@@ -7132,7 +7132,7 @@
         <v>0</v>
       </c>
       <c r="K191" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="192">
@@ -7167,7 +7167,7 @@
         <v>1</v>
       </c>
       <c r="K192" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="193">
@@ -7202,7 +7202,7 @@
         <v>0</v>
       </c>
       <c r="K193" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="194">
@@ -7237,7 +7237,7 @@
         <v>1</v>
       </c>
       <c r="K194" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="195">
@@ -7272,7 +7272,7 @@
         <v>0</v>
       </c>
       <c r="K195" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="196">
@@ -7307,7 +7307,7 @@
         <v>0</v>
       </c>
       <c r="K196" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="197">
@@ -7342,7 +7342,7 @@
         <v>0</v>
       </c>
       <c r="K197" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="198">
@@ -7412,7 +7412,7 @@
         <v>0</v>
       </c>
       <c r="K199" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="200">
@@ -7447,7 +7447,7 @@
         <v>1</v>
       </c>
       <c r="K200" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="201">
@@ -7482,7 +7482,7 @@
         <v>0</v>
       </c>
       <c r="K201" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="202">
@@ -7552,7 +7552,7 @@
         <v>0</v>
       </c>
       <c r="K203" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="204">
@@ -7622,7 +7622,7 @@
         <v>0</v>
       </c>
       <c r="K205" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="206">
@@ -7657,7 +7657,7 @@
         <v>0</v>
       </c>
       <c r="K206" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="207">
@@ -7692,7 +7692,7 @@
         <v>1</v>
       </c>
       <c r="K207" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="208">
@@ -7727,7 +7727,7 @@
         <v>0</v>
       </c>
       <c r="K208" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="209">
@@ -7762,7 +7762,7 @@
         <v>1</v>
       </c>
       <c r="K209" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="210">
@@ -7797,7 +7797,7 @@
         <v>0</v>
       </c>
       <c r="K210" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="211">
@@ -7832,7 +7832,7 @@
         <v>0</v>
       </c>
       <c r="K211" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="212">
@@ -7867,7 +7867,7 @@
         <v>0</v>
       </c>
       <c r="K212" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="213">
@@ -7937,7 +7937,7 @@
         <v>0</v>
       </c>
       <c r="K214" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="215">
@@ -7972,7 +7972,7 @@
         <v>1</v>
       </c>
       <c r="K215" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="216">
@@ -8007,7 +8007,7 @@
         <v>0</v>
       </c>
       <c r="K216" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="217">
@@ -8077,7 +8077,7 @@
         <v>0</v>
       </c>
       <c r="K218" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="219">
@@ -8147,7 +8147,7 @@
         <v>0</v>
       </c>
       <c r="K220" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="221">
@@ -8182,7 +8182,7 @@
         <v>0</v>
       </c>
       <c r="K221" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="222">
@@ -8217,7 +8217,7 @@
         <v>1</v>
       </c>
       <c r="K222" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="223">
@@ -8252,7 +8252,7 @@
         <v>0</v>
       </c>
       <c r="K223" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="224">
@@ -8287,7 +8287,7 @@
         <v>1</v>
       </c>
       <c r="K224" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="225">
@@ -8322,7 +8322,7 @@
         <v>0</v>
       </c>
       <c r="K225" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="226">
@@ -8357,7 +8357,7 @@
         <v>0</v>
       </c>
       <c r="K226" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="227">
@@ -8392,7 +8392,7 @@
         <v>0</v>
       </c>
       <c r="K227" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="228">
@@ -8462,7 +8462,7 @@
         <v>0</v>
       </c>
       <c r="K229" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="230">
@@ -8497,7 +8497,7 @@
         <v>1</v>
       </c>
       <c r="K230" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="231">
@@ -8532,7 +8532,7 @@
         <v>0</v>
       </c>
       <c r="K231" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="232">
@@ -8602,7 +8602,7 @@
         <v>0</v>
       </c>
       <c r="K233" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="234">
@@ -8672,7 +8672,7 @@
         <v>0</v>
       </c>
       <c r="K235" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="236">
@@ -8707,7 +8707,7 @@
         <v>0</v>
       </c>
       <c r="K236" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="237">
@@ -8742,7 +8742,7 @@
         <v>1</v>
       </c>
       <c r="K237" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="238">
@@ -8777,7 +8777,7 @@
         <v>0</v>
       </c>
       <c r="K238" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="239">
@@ -8812,7 +8812,7 @@
         <v>1</v>
       </c>
       <c r="K239" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="240">
@@ -8847,7 +8847,7 @@
         <v>0</v>
       </c>
       <c r="K240" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="241">
@@ -8882,7 +8882,7 @@
         <v>0</v>
       </c>
       <c r="K241" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="242">
@@ -8917,7 +8917,7 @@
         <v>0</v>
       </c>
       <c r="K242" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="243">
@@ -8987,7 +8987,7 @@
         <v>0</v>
       </c>
       <c r="K244" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="245">
@@ -9022,7 +9022,7 @@
         <v>1</v>
       </c>
       <c r="K245" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="246">
@@ -9057,7 +9057,7 @@
         <v>0</v>
       </c>
       <c r="K246" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="247">
@@ -9127,7 +9127,7 @@
         <v>0</v>
       </c>
       <c r="K248" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="249">
@@ -9197,7 +9197,7 @@
         <v>0</v>
       </c>
       <c r="K250" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="251">
@@ -9232,7 +9232,7 @@
         <v>0</v>
       </c>
       <c r="K251" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="252">
@@ -9267,7 +9267,7 @@
         <v>1</v>
       </c>
       <c r="K252" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="253">
@@ -9302,7 +9302,7 @@
         <v>0</v>
       </c>
       <c r="K253" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="254">
@@ -9337,7 +9337,7 @@
         <v>1</v>
       </c>
       <c r="K254" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="255">
@@ -9372,7 +9372,7 @@
         <v>0</v>
       </c>
       <c r="K255" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="256">
@@ -9407,7 +9407,7 @@
         <v>0</v>
       </c>
       <c r="K256" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="257">
@@ -9442,7 +9442,7 @@
         <v>0</v>
       </c>
       <c r="K257" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="258">
@@ -9512,7 +9512,7 @@
         <v>0</v>
       </c>
       <c r="K259" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="260">
@@ -9547,7 +9547,7 @@
         <v>1</v>
       </c>
       <c r="K260" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="261">
@@ -9582,7 +9582,7 @@
         <v>0</v>
       </c>
       <c r="K261" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="262">
@@ -9652,7 +9652,7 @@
         <v>0</v>
       </c>
       <c r="K263" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="264">
@@ -9722,7 +9722,7 @@
         <v>0</v>
       </c>
       <c r="K265" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="266">
@@ -9757,7 +9757,7 @@
         <v>0</v>
       </c>
       <c r="K266" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="267">
@@ -9792,7 +9792,7 @@
         <v>1</v>
       </c>
       <c r="K267" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="268">
@@ -9827,7 +9827,7 @@
         <v>0</v>
       </c>
       <c r="K268" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="269">
@@ -9862,7 +9862,7 @@
         <v>1</v>
       </c>
       <c r="K269" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="270">
@@ -9897,7 +9897,7 @@
         <v>0</v>
       </c>
       <c r="K270" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="271">
@@ -9932,7 +9932,7 @@
         <v>0</v>
       </c>
       <c r="K271" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Navegación entre ventanas lista y funcionamiento de la lista de empresas con su lista de empleados funcionando parcialmente, falta agregar que se actualice cada que se agrega un empleado
</commit_message>
<xml_diff>
--- a/clustersEmpleados.xlsx
+++ b/clustersEmpleados.xlsx
@@ -552,7 +552,7 @@
         <v>1</v>
       </c>
       <c r="K3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -587,7 +587,7 @@
         <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -622,7 +622,7 @@
         <v>1</v>
       </c>
       <c r="K5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -657,7 +657,7 @@
         <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -692,7 +692,7 @@
         <v>1</v>
       </c>
       <c r="K7" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -727,7 +727,7 @@
         <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9">
@@ -762,7 +762,7 @@
         <v>1</v>
       </c>
       <c r="K9" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -797,7 +797,7 @@
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -832,7 +832,7 @@
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -867,7 +867,7 @@
         <v>1</v>
       </c>
       <c r="K12" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13">
@@ -902,7 +902,7 @@
         <v>0</v>
       </c>
       <c r="K13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -937,7 +937,7 @@
         <v>1</v>
       </c>
       <c r="K14" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15">
@@ -972,7 +972,7 @@
         <v>0</v>
       </c>
       <c r="K15" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16">
@@ -1007,7 +1007,7 @@
         <v>0</v>
       </c>
       <c r="K16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
@@ -1077,7 +1077,7 @@
         <v>1</v>
       </c>
       <c r="K18" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -1112,7 +1112,7 @@
         <v>0</v>
       </c>
       <c r="K19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -1147,7 +1147,7 @@
         <v>1</v>
       </c>
       <c r="K20" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21">
@@ -1182,7 +1182,7 @@
         <v>0</v>
       </c>
       <c r="K21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -1217,7 +1217,7 @@
         <v>1</v>
       </c>
       <c r="K22" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -1252,7 +1252,7 @@
         <v>0</v>
       </c>
       <c r="K23" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24">
@@ -1287,7 +1287,7 @@
         <v>1</v>
       </c>
       <c r="K24" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1322,7 +1322,7 @@
         <v>0</v>
       </c>
       <c r="K25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -1357,7 +1357,7 @@
         <v>0</v>
       </c>
       <c r="K26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -1392,7 +1392,7 @@
         <v>1</v>
       </c>
       <c r="K27" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28">
@@ -1427,7 +1427,7 @@
         <v>0</v>
       </c>
       <c r="K28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
@@ -1462,7 +1462,7 @@
         <v>1</v>
       </c>
       <c r="K29" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30">
@@ -1497,7 +1497,7 @@
         <v>0</v>
       </c>
       <c r="K30" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31">
@@ -1532,7 +1532,7 @@
         <v>0</v>
       </c>
       <c r="K31" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32">
@@ -1602,7 +1602,7 @@
         <v>1</v>
       </c>
       <c r="K33" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -1637,7 +1637,7 @@
         <v>0</v>
       </c>
       <c r="K34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
@@ -1672,7 +1672,7 @@
         <v>1</v>
       </c>
       <c r="K35" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36">
@@ -1707,7 +1707,7 @@
         <v>0</v>
       </c>
       <c r="K36" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
@@ -1742,7 +1742,7 @@
         <v>1</v>
       </c>
       <c r="K37" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -1777,7 +1777,7 @@
         <v>0</v>
       </c>
       <c r="K38" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39">
@@ -1812,7 +1812,7 @@
         <v>1</v>
       </c>
       <c r="K39" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -1847,7 +1847,7 @@
         <v>0</v>
       </c>
       <c r="K40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
@@ -1882,7 +1882,7 @@
         <v>0</v>
       </c>
       <c r="K41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -1917,7 +1917,7 @@
         <v>1</v>
       </c>
       <c r="K42" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43">
@@ -1952,7 +1952,7 @@
         <v>0</v>
       </c>
       <c r="K43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44">
@@ -1987,7 +1987,7 @@
         <v>1</v>
       </c>
       <c r="K44" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45">
@@ -2022,7 +2022,7 @@
         <v>0</v>
       </c>
       <c r="K45" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46">
@@ -2057,7 +2057,7 @@
         <v>0</v>
       </c>
       <c r="K46" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47">
@@ -2127,7 +2127,7 @@
         <v>1</v>
       </c>
       <c r="K48" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -2162,7 +2162,7 @@
         <v>0</v>
       </c>
       <c r="K49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50">
@@ -2197,7 +2197,7 @@
         <v>1</v>
       </c>
       <c r="K50" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51">
@@ -2232,7 +2232,7 @@
         <v>0</v>
       </c>
       <c r="K51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52">
@@ -2267,7 +2267,7 @@
         <v>1</v>
       </c>
       <c r="K52" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -2302,7 +2302,7 @@
         <v>0</v>
       </c>
       <c r="K53" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54">
@@ -2337,7 +2337,7 @@
         <v>1</v>
       </c>
       <c r="K54" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -2372,7 +2372,7 @@
         <v>0</v>
       </c>
       <c r="K55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56">
@@ -2407,7 +2407,7 @@
         <v>0</v>
       </c>
       <c r="K56" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57">
@@ -2442,7 +2442,7 @@
         <v>1</v>
       </c>
       <c r="K57" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58">
@@ -2477,7 +2477,7 @@
         <v>0</v>
       </c>
       <c r="K58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59">
@@ -2512,7 +2512,7 @@
         <v>1</v>
       </c>
       <c r="K59" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60">
@@ -2547,7 +2547,7 @@
         <v>0</v>
       </c>
       <c r="K60" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61">
@@ -2582,7 +2582,7 @@
         <v>0</v>
       </c>
       <c r="K61" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62">
@@ -2652,7 +2652,7 @@
         <v>1</v>
       </c>
       <c r="K63" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -2687,7 +2687,7 @@
         <v>0</v>
       </c>
       <c r="K64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65">
@@ -2722,7 +2722,7 @@
         <v>1</v>
       </c>
       <c r="K65" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="66">
@@ -2757,7 +2757,7 @@
         <v>0</v>
       </c>
       <c r="K66" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67">
@@ -2792,7 +2792,7 @@
         <v>1</v>
       </c>
       <c r="K67" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -2827,7 +2827,7 @@
         <v>0</v>
       </c>
       <c r="K68" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="69">
@@ -2862,7 +2862,7 @@
         <v>1</v>
       </c>
       <c r="K69" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -2897,7 +2897,7 @@
         <v>0</v>
       </c>
       <c r="K70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71">
@@ -2932,7 +2932,7 @@
         <v>0</v>
       </c>
       <c r="K71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72">
@@ -2967,7 +2967,7 @@
         <v>1</v>
       </c>
       <c r="K72" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="73">
@@ -3002,7 +3002,7 @@
         <v>0</v>
       </c>
       <c r="K73" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74">
@@ -3037,7 +3037,7 @@
         <v>1</v>
       </c>
       <c r="K74" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75">
@@ -3072,7 +3072,7 @@
         <v>0</v>
       </c>
       <c r="K75" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76">
@@ -3107,7 +3107,7 @@
         <v>0</v>
       </c>
       <c r="K76" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77">
@@ -3177,7 +3177,7 @@
         <v>1</v>
       </c>
       <c r="K78" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79">
@@ -3212,7 +3212,7 @@
         <v>0</v>
       </c>
       <c r="K79" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80">
@@ -3247,7 +3247,7 @@
         <v>1</v>
       </c>
       <c r="K80" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="81">
@@ -3282,7 +3282,7 @@
         <v>0</v>
       </c>
       <c r="K81" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82">
@@ -3317,7 +3317,7 @@
         <v>1</v>
       </c>
       <c r="K82" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83">
@@ -3352,7 +3352,7 @@
         <v>0</v>
       </c>
       <c r="K83" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="84">
@@ -3387,7 +3387,7 @@
         <v>1</v>
       </c>
       <c r="K84" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85">
@@ -3422,7 +3422,7 @@
         <v>0</v>
       </c>
       <c r="K85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86">
@@ -3457,7 +3457,7 @@
         <v>0</v>
       </c>
       <c r="K86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87">
@@ -3492,7 +3492,7 @@
         <v>1</v>
       </c>
       <c r="K87" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="88">
@@ -3527,7 +3527,7 @@
         <v>0</v>
       </c>
       <c r="K88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89">
@@ -3562,7 +3562,7 @@
         <v>1</v>
       </c>
       <c r="K89" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="90">
@@ -3597,7 +3597,7 @@
         <v>0</v>
       </c>
       <c r="K90" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="91">
@@ -3632,7 +3632,7 @@
         <v>0</v>
       </c>
       <c r="K91" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="92">
@@ -3702,7 +3702,7 @@
         <v>1</v>
       </c>
       <c r="K93" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94">
@@ -3737,7 +3737,7 @@
         <v>0</v>
       </c>
       <c r="K94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95">
@@ -3772,7 +3772,7 @@
         <v>1</v>
       </c>
       <c r="K95" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="96">
@@ -3807,7 +3807,7 @@
         <v>0</v>
       </c>
       <c r="K96" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97">
@@ -3842,7 +3842,7 @@
         <v>1</v>
       </c>
       <c r="K97" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98">
@@ -3877,7 +3877,7 @@
         <v>0</v>
       </c>
       <c r="K98" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="99">
@@ -3912,7 +3912,7 @@
         <v>1</v>
       </c>
       <c r="K99" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100">
@@ -3947,7 +3947,7 @@
         <v>0</v>
       </c>
       <c r="K100" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101">
@@ -3982,7 +3982,7 @@
         <v>0</v>
       </c>
       <c r="K101" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102">
@@ -4017,7 +4017,7 @@
         <v>1</v>
       </c>
       <c r="K102" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="103">
@@ -4052,7 +4052,7 @@
         <v>0</v>
       </c>
       <c r="K103" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104">
@@ -4087,7 +4087,7 @@
         <v>1</v>
       </c>
       <c r="K104" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="105">
@@ -4122,7 +4122,7 @@
         <v>0</v>
       </c>
       <c r="K105" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="106">
@@ -4157,7 +4157,7 @@
         <v>0</v>
       </c>
       <c r="K106" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="107">
@@ -4227,7 +4227,7 @@
         <v>1</v>
       </c>
       <c r="K108" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109">
@@ -4262,7 +4262,7 @@
         <v>0</v>
       </c>
       <c r="K109" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110">
@@ -4297,7 +4297,7 @@
         <v>1</v>
       </c>
       <c r="K110" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="111">
@@ -4332,7 +4332,7 @@
         <v>0</v>
       </c>
       <c r="K111" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112">
@@ -4367,7 +4367,7 @@
         <v>1</v>
       </c>
       <c r="K112" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113">
@@ -4402,7 +4402,7 @@
         <v>0</v>
       </c>
       <c r="K113" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="114">
@@ -4437,7 +4437,7 @@
         <v>1</v>
       </c>
       <c r="K114" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115">
@@ -4472,7 +4472,7 @@
         <v>0</v>
       </c>
       <c r="K115" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116">
@@ -4507,7 +4507,7 @@
         <v>0</v>
       </c>
       <c r="K116" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117">
@@ -4542,7 +4542,7 @@
         <v>1</v>
       </c>
       <c r="K117" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="118">
@@ -4577,7 +4577,7 @@
         <v>0</v>
       </c>
       <c r="K118" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119">
@@ -4612,7 +4612,7 @@
         <v>1</v>
       </c>
       <c r="K119" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="120">
@@ -4647,7 +4647,7 @@
         <v>0</v>
       </c>
       <c r="K120" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="121">
@@ -4682,7 +4682,7 @@
         <v>0</v>
       </c>
       <c r="K121" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="122">
@@ -4752,7 +4752,7 @@
         <v>1</v>
       </c>
       <c r="K123" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124">
@@ -4787,7 +4787,7 @@
         <v>0</v>
       </c>
       <c r="K124" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125">
@@ -4822,7 +4822,7 @@
         <v>1</v>
       </c>
       <c r="K125" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="126">
@@ -4857,7 +4857,7 @@
         <v>0</v>
       </c>
       <c r="K126" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127">
@@ -4892,7 +4892,7 @@
         <v>1</v>
       </c>
       <c r="K127" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128">
@@ -4927,7 +4927,7 @@
         <v>0</v>
       </c>
       <c r="K128" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="129">
@@ -4962,7 +4962,7 @@
         <v>1</v>
       </c>
       <c r="K129" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130">
@@ -4997,7 +4997,7 @@
         <v>0</v>
       </c>
       <c r="K130" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131">
@@ -5032,7 +5032,7 @@
         <v>0</v>
       </c>
       <c r="K131" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132">
@@ -5067,7 +5067,7 @@
         <v>1</v>
       </c>
       <c r="K132" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="133">
@@ -5102,7 +5102,7 @@
         <v>0</v>
       </c>
       <c r="K133" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134">
@@ -5137,7 +5137,7 @@
         <v>1</v>
       </c>
       <c r="K134" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="135">
@@ -5172,7 +5172,7 @@
         <v>0</v>
       </c>
       <c r="K135" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="136">
@@ -5207,7 +5207,7 @@
         <v>0</v>
       </c>
       <c r="K136" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="137">
@@ -5277,7 +5277,7 @@
         <v>1</v>
       </c>
       <c r="K138" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139">
@@ -5312,7 +5312,7 @@
         <v>0</v>
       </c>
       <c r="K139" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140">
@@ -5347,7 +5347,7 @@
         <v>1</v>
       </c>
       <c r="K140" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="141">
@@ -5382,7 +5382,7 @@
         <v>0</v>
       </c>
       <c r="K141" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142">
@@ -5417,7 +5417,7 @@
         <v>1</v>
       </c>
       <c r="K142" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143">
@@ -5452,7 +5452,7 @@
         <v>0</v>
       </c>
       <c r="K143" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="144">
@@ -5487,7 +5487,7 @@
         <v>1</v>
       </c>
       <c r="K144" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145">
@@ -5522,7 +5522,7 @@
         <v>0</v>
       </c>
       <c r="K145" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146">
@@ -5557,7 +5557,7 @@
         <v>0</v>
       </c>
       <c r="K146" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147">
@@ -5592,7 +5592,7 @@
         <v>1</v>
       </c>
       <c r="K147" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="148">
@@ -5627,7 +5627,7 @@
         <v>0</v>
       </c>
       <c r="K148" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149">
@@ -5662,7 +5662,7 @@
         <v>1</v>
       </c>
       <c r="K149" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="150">
@@ -5697,7 +5697,7 @@
         <v>0</v>
       </c>
       <c r="K150" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="151">
@@ -5732,7 +5732,7 @@
         <v>0</v>
       </c>
       <c r="K151" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="152">
@@ -5802,7 +5802,7 @@
         <v>1</v>
       </c>
       <c r="K153" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154">
@@ -5837,7 +5837,7 @@
         <v>0</v>
       </c>
       <c r="K154" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155">
@@ -5872,7 +5872,7 @@
         <v>1</v>
       </c>
       <c r="K155" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="156">
@@ -5907,7 +5907,7 @@
         <v>0</v>
       </c>
       <c r="K156" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157">
@@ -5942,7 +5942,7 @@
         <v>1</v>
       </c>
       <c r="K157" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158">
@@ -5977,7 +5977,7 @@
         <v>0</v>
       </c>
       <c r="K158" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="159">
@@ -6012,7 +6012,7 @@
         <v>1</v>
       </c>
       <c r="K159" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="160">
@@ -6047,7 +6047,7 @@
         <v>0</v>
       </c>
       <c r="K160" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161">
@@ -6082,7 +6082,7 @@
         <v>0</v>
       </c>
       <c r="K161" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="162">
@@ -6117,7 +6117,7 @@
         <v>1</v>
       </c>
       <c r="K162" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="163">
@@ -6152,7 +6152,7 @@
         <v>0</v>
       </c>
       <c r="K163" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164">
@@ -6187,7 +6187,7 @@
         <v>1</v>
       </c>
       <c r="K164" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="165">
@@ -6222,7 +6222,7 @@
         <v>0</v>
       </c>
       <c r="K165" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="166">
@@ -6257,7 +6257,7 @@
         <v>0</v>
       </c>
       <c r="K166" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="167">
@@ -6327,7 +6327,7 @@
         <v>1</v>
       </c>
       <c r="K168" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="169">
@@ -6362,7 +6362,7 @@
         <v>0</v>
       </c>
       <c r="K169" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="170">
@@ -6397,7 +6397,7 @@
         <v>1</v>
       </c>
       <c r="K170" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="171">
@@ -6432,7 +6432,7 @@
         <v>0</v>
       </c>
       <c r="K171" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="172">
@@ -6467,7 +6467,7 @@
         <v>1</v>
       </c>
       <c r="K172" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="173">
@@ -6502,7 +6502,7 @@
         <v>0</v>
       </c>
       <c r="K173" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="174">
@@ -6537,7 +6537,7 @@
         <v>1</v>
       </c>
       <c r="K174" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="175">
@@ -6572,7 +6572,7 @@
         <v>0</v>
       </c>
       <c r="K175" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="176">
@@ -6607,7 +6607,7 @@
         <v>0</v>
       </c>
       <c r="K176" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177">
@@ -6642,7 +6642,7 @@
         <v>1</v>
       </c>
       <c r="K177" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="178">
@@ -6677,7 +6677,7 @@
         <v>0</v>
       </c>
       <c r="K178" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="179">
@@ -6712,7 +6712,7 @@
         <v>1</v>
       </c>
       <c r="K179" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="180">
@@ -6747,7 +6747,7 @@
         <v>0</v>
       </c>
       <c r="K180" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="181">
@@ -6782,7 +6782,7 @@
         <v>0</v>
       </c>
       <c r="K181" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="182">
@@ -6852,7 +6852,7 @@
         <v>1</v>
       </c>
       <c r="K183" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="184">
@@ -6887,7 +6887,7 @@
         <v>0</v>
       </c>
       <c r="K184" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="185">
@@ -6922,7 +6922,7 @@
         <v>1</v>
       </c>
       <c r="K185" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="186">
@@ -6957,7 +6957,7 @@
         <v>0</v>
       </c>
       <c r="K186" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="187">
@@ -6992,7 +6992,7 @@
         <v>1</v>
       </c>
       <c r="K187" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="188">
@@ -7027,7 +7027,7 @@
         <v>0</v>
       </c>
       <c r="K188" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="189">
@@ -7062,7 +7062,7 @@
         <v>1</v>
       </c>
       <c r="K189" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="190">
@@ -7097,7 +7097,7 @@
         <v>0</v>
       </c>
       <c r="K190" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="191">
@@ -7132,7 +7132,7 @@
         <v>0</v>
       </c>
       <c r="K191" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="192">
@@ -7167,7 +7167,7 @@
         <v>1</v>
       </c>
       <c r="K192" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="193">
@@ -7202,7 +7202,7 @@
         <v>0</v>
       </c>
       <c r="K193" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="194">
@@ -7237,7 +7237,7 @@
         <v>1</v>
       </c>
       <c r="K194" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="195">
@@ -7272,7 +7272,7 @@
         <v>0</v>
       </c>
       <c r="K195" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="196">
@@ -7307,7 +7307,7 @@
         <v>0</v>
       </c>
       <c r="K196" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="197">
@@ -7377,7 +7377,7 @@
         <v>1</v>
       </c>
       <c r="K198" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="199">
@@ -7412,7 +7412,7 @@
         <v>0</v>
       </c>
       <c r="K199" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="200">
@@ -7447,7 +7447,7 @@
         <v>1</v>
       </c>
       <c r="K200" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="201">
@@ -7482,7 +7482,7 @@
         <v>0</v>
       </c>
       <c r="K201" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="202">
@@ -7517,7 +7517,7 @@
         <v>1</v>
       </c>
       <c r="K202" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="203">
@@ -7552,7 +7552,7 @@
         <v>0</v>
       </c>
       <c r="K203" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="204">
@@ -7587,7 +7587,7 @@
         <v>1</v>
       </c>
       <c r="K204" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="205">
@@ -7622,7 +7622,7 @@
         <v>0</v>
       </c>
       <c r="K205" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="206">
@@ -7657,7 +7657,7 @@
         <v>0</v>
       </c>
       <c r="K206" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="207">
@@ -7692,7 +7692,7 @@
         <v>1</v>
       </c>
       <c r="K207" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="208">
@@ -7727,7 +7727,7 @@
         <v>0</v>
       </c>
       <c r="K208" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="209">
@@ -7762,7 +7762,7 @@
         <v>1</v>
       </c>
       <c r="K209" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="210">
@@ -7797,7 +7797,7 @@
         <v>0</v>
       </c>
       <c r="K210" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="211">
@@ -7832,7 +7832,7 @@
         <v>0</v>
       </c>
       <c r="K211" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="212">
@@ -7902,7 +7902,7 @@
         <v>1</v>
       </c>
       <c r="K213" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="214">
@@ -7937,7 +7937,7 @@
         <v>0</v>
       </c>
       <c r="K214" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="215">
@@ -7972,7 +7972,7 @@
         <v>1</v>
       </c>
       <c r="K215" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="216">
@@ -8007,7 +8007,7 @@
         <v>0</v>
       </c>
       <c r="K216" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="217">
@@ -8042,7 +8042,7 @@
         <v>1</v>
       </c>
       <c r="K217" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="218">
@@ -8077,7 +8077,7 @@
         <v>0</v>
       </c>
       <c r="K218" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="219">
@@ -8112,7 +8112,7 @@
         <v>1</v>
       </c>
       <c r="K219" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="220">
@@ -8147,7 +8147,7 @@
         <v>0</v>
       </c>
       <c r="K220" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="221">
@@ -8182,7 +8182,7 @@
         <v>0</v>
       </c>
       <c r="K221" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="222">
@@ -8217,7 +8217,7 @@
         <v>1</v>
       </c>
       <c r="K222" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="223">
@@ -8252,7 +8252,7 @@
         <v>0</v>
       </c>
       <c r="K223" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="224">
@@ -8287,7 +8287,7 @@
         <v>1</v>
       </c>
       <c r="K224" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="225">
@@ -8322,7 +8322,7 @@
         <v>0</v>
       </c>
       <c r="K225" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="226">
@@ -8357,7 +8357,7 @@
         <v>0</v>
       </c>
       <c r="K226" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="227">
@@ -8427,7 +8427,7 @@
         <v>1</v>
       </c>
       <c r="K228" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="229">
@@ -8462,7 +8462,7 @@
         <v>0</v>
       </c>
       <c r="K229" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="230">
@@ -8497,7 +8497,7 @@
         <v>1</v>
       </c>
       <c r="K230" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="231">
@@ -8532,7 +8532,7 @@
         <v>0</v>
       </c>
       <c r="K231" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="232">
@@ -8567,7 +8567,7 @@
         <v>1</v>
       </c>
       <c r="K232" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="233">
@@ -8602,7 +8602,7 @@
         <v>0</v>
       </c>
       <c r="K233" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="234">
@@ -8637,7 +8637,7 @@
         <v>1</v>
       </c>
       <c r="K234" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="235">
@@ -8672,7 +8672,7 @@
         <v>0</v>
       </c>
       <c r="K235" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="236">
@@ -8707,7 +8707,7 @@
         <v>0</v>
       </c>
       <c r="K236" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="237">
@@ -8742,7 +8742,7 @@
         <v>1</v>
       </c>
       <c r="K237" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="238">
@@ -8777,7 +8777,7 @@
         <v>0</v>
       </c>
       <c r="K238" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="239">
@@ -8812,7 +8812,7 @@
         <v>1</v>
       </c>
       <c r="K239" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="240">
@@ -8847,7 +8847,7 @@
         <v>0</v>
       </c>
       <c r="K240" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="241">
@@ -8882,7 +8882,7 @@
         <v>0</v>
       </c>
       <c r="K241" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="242">
@@ -8952,7 +8952,7 @@
         <v>1</v>
       </c>
       <c r="K243" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="244">
@@ -8987,7 +8987,7 @@
         <v>0</v>
       </c>
       <c r="K244" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="245">
@@ -9022,7 +9022,7 @@
         <v>1</v>
       </c>
       <c r="K245" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="246">
@@ -9057,7 +9057,7 @@
         <v>0</v>
       </c>
       <c r="K246" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="247">
@@ -9092,7 +9092,7 @@
         <v>1</v>
       </c>
       <c r="K247" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="248">
@@ -9127,7 +9127,7 @@
         <v>0</v>
       </c>
       <c r="K248" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="249">
@@ -9162,7 +9162,7 @@
         <v>1</v>
       </c>
       <c r="K249" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="250">
@@ -9197,7 +9197,7 @@
         <v>0</v>
       </c>
       <c r="K250" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="251">
@@ -9232,7 +9232,7 @@
         <v>0</v>
       </c>
       <c r="K251" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="252">
@@ -9267,7 +9267,7 @@
         <v>1</v>
       </c>
       <c r="K252" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="253">
@@ -9302,7 +9302,7 @@
         <v>0</v>
       </c>
       <c r="K253" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="254">
@@ -9337,7 +9337,7 @@
         <v>1</v>
       </c>
       <c r="K254" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="255">
@@ -9372,7 +9372,7 @@
         <v>0</v>
       </c>
       <c r="K255" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="256">
@@ -9407,7 +9407,7 @@
         <v>0</v>
       </c>
       <c r="K256" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="257">
@@ -9477,7 +9477,7 @@
         <v>1</v>
       </c>
       <c r="K258" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="259">
@@ -9512,7 +9512,7 @@
         <v>0</v>
       </c>
       <c r="K259" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="260">
@@ -9547,7 +9547,7 @@
         <v>1</v>
       </c>
       <c r="K260" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="261">
@@ -9582,7 +9582,7 @@
         <v>0</v>
       </c>
       <c r="K261" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="262">
@@ -9617,7 +9617,7 @@
         <v>1</v>
       </c>
       <c r="K262" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="263">
@@ -9652,7 +9652,7 @@
         <v>0</v>
       </c>
       <c r="K263" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="264">
@@ -9687,7 +9687,7 @@
         <v>1</v>
       </c>
       <c r="K264" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="265">
@@ -9722,7 +9722,7 @@
         <v>0</v>
       </c>
       <c r="K265" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="266">
@@ -9757,7 +9757,7 @@
         <v>0</v>
       </c>
       <c r="K266" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="267">
@@ -9792,7 +9792,7 @@
         <v>1</v>
       </c>
       <c r="K267" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="268">
@@ -9827,7 +9827,7 @@
         <v>0</v>
       </c>
       <c r="K268" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="269">
@@ -9862,7 +9862,7 @@
         <v>1</v>
       </c>
       <c r="K269" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="270">
@@ -9897,7 +9897,7 @@
         <v>0</v>
       </c>
       <c r="K270" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="271">
@@ -9932,7 +9932,7 @@
         <v>0</v>
       </c>
       <c r="K271" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Funcionalidad y navegación de editar nomina listo, ademas de la función de agregar empleado implementada.
</commit_message>
<xml_diff>
--- a/clustersEmpleados.xlsx
+++ b/clustersEmpleados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K271"/>
+  <dimension ref="A1:K272"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,7 +517,7 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -552,7 +552,7 @@
         <v>1</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -692,7 +692,7 @@
         <v>1</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
@@ -762,7 +762,7 @@
         <v>1</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
@@ -972,7 +972,7 @@
         <v>0</v>
       </c>
       <c r="K15" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16">
@@ -1007,7 +1007,7 @@
         <v>0</v>
       </c>
       <c r="K16" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17">
@@ -1042,7 +1042,7 @@
         <v>0</v>
       </c>
       <c r="K17" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -1077,7 +1077,7 @@
         <v>1</v>
       </c>
       <c r="K18" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">
@@ -1217,7 +1217,7 @@
         <v>1</v>
       </c>
       <c r="K22" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
@@ -1287,7 +1287,7 @@
         <v>1</v>
       </c>
       <c r="K24" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
@@ -1497,7 +1497,7 @@
         <v>0</v>
       </c>
       <c r="K30" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31">
@@ -1532,7 +1532,7 @@
         <v>0</v>
       </c>
       <c r="K31" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32">
@@ -1567,7 +1567,7 @@
         <v>0</v>
       </c>
       <c r="K32" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -1602,7 +1602,7 @@
         <v>1</v>
       </c>
       <c r="K33" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34">
@@ -1742,7 +1742,7 @@
         <v>1</v>
       </c>
       <c r="K37" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38">
@@ -1812,7 +1812,7 @@
         <v>1</v>
       </c>
       <c r="K39" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40">
@@ -2022,7 +2022,7 @@
         <v>0</v>
       </c>
       <c r="K45" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46">
@@ -2057,7 +2057,7 @@
         <v>0</v>
       </c>
       <c r="K46" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47">
@@ -2092,7 +2092,7 @@
         <v>0</v>
       </c>
       <c r="K47" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -2127,7 +2127,7 @@
         <v>1</v>
       </c>
       <c r="K48" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49">
@@ -2267,7 +2267,7 @@
         <v>1</v>
       </c>
       <c r="K52" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53">
@@ -2337,7 +2337,7 @@
         <v>1</v>
       </c>
       <c r="K54" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55">
@@ -2547,7 +2547,7 @@
         <v>0</v>
       </c>
       <c r="K60" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61">
@@ -2582,7 +2582,7 @@
         <v>0</v>
       </c>
       <c r="K61" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="62">
@@ -2617,7 +2617,7 @@
         <v>0</v>
       </c>
       <c r="K62" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -2652,7 +2652,7 @@
         <v>1</v>
       </c>
       <c r="K63" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64">
@@ -2792,7 +2792,7 @@
         <v>1</v>
       </c>
       <c r="K67" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68">
@@ -2862,7 +2862,7 @@
         <v>1</v>
       </c>
       <c r="K69" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70">
@@ -3072,7 +3072,7 @@
         <v>0</v>
       </c>
       <c r="K75" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="76">
@@ -3107,7 +3107,7 @@
         <v>0</v>
       </c>
       <c r="K76" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="77">
@@ -3142,7 +3142,7 @@
         <v>0</v>
       </c>
       <c r="K77" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78">
@@ -3177,7 +3177,7 @@
         <v>1</v>
       </c>
       <c r="K78" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79">
@@ -3317,7 +3317,7 @@
         <v>1</v>
       </c>
       <c r="K82" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83">
@@ -3387,7 +3387,7 @@
         <v>1</v>
       </c>
       <c r="K84" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85">
@@ -3597,7 +3597,7 @@
         <v>0</v>
       </c>
       <c r="K90" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="91">
@@ -3632,7 +3632,7 @@
         <v>0</v>
       </c>
       <c r="K91" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="92">
@@ -3667,7 +3667,7 @@
         <v>0</v>
       </c>
       <c r="K92" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93">
@@ -3702,7 +3702,7 @@
         <v>1</v>
       </c>
       <c r="K93" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94">
@@ -3842,7 +3842,7 @@
         <v>1</v>
       </c>
       <c r="K97" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="98">
@@ -3912,7 +3912,7 @@
         <v>1</v>
       </c>
       <c r="K99" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="100">
@@ -4122,7 +4122,7 @@
         <v>0</v>
       </c>
       <c r="K105" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="106">
@@ -4157,7 +4157,7 @@
         <v>0</v>
       </c>
       <c r="K106" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="107">
@@ -4192,7 +4192,7 @@
         <v>0</v>
       </c>
       <c r="K107" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108">
@@ -4227,7 +4227,7 @@
         <v>1</v>
       </c>
       <c r="K108" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="109">
@@ -4367,7 +4367,7 @@
         <v>1</v>
       </c>
       <c r="K112" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113">
@@ -4437,7 +4437,7 @@
         <v>1</v>
       </c>
       <c r="K114" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="115">
@@ -4647,7 +4647,7 @@
         <v>0</v>
       </c>
       <c r="K120" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="121">
@@ -4682,7 +4682,7 @@
         <v>0</v>
       </c>
       <c r="K121" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="122">
@@ -4717,7 +4717,7 @@
         <v>0</v>
       </c>
       <c r="K122" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123">
@@ -4752,7 +4752,7 @@
         <v>1</v>
       </c>
       <c r="K123" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="124">
@@ -4892,7 +4892,7 @@
         <v>1</v>
       </c>
       <c r="K127" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="128">
@@ -4962,7 +4962,7 @@
         <v>1</v>
       </c>
       <c r="K129" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="130">
@@ -5172,7 +5172,7 @@
         <v>0</v>
       </c>
       <c r="K135" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="136">
@@ -5207,7 +5207,7 @@
         <v>0</v>
       </c>
       <c r="K136" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="137">
@@ -5242,7 +5242,7 @@
         <v>0</v>
       </c>
       <c r="K137" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138">
@@ -5277,7 +5277,7 @@
         <v>1</v>
       </c>
       <c r="K138" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="139">
@@ -5417,7 +5417,7 @@
         <v>1</v>
       </c>
       <c r="K142" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="143">
@@ -5487,7 +5487,7 @@
         <v>1</v>
       </c>
       <c r="K144" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="145">
@@ -5697,7 +5697,7 @@
         <v>0</v>
       </c>
       <c r="K150" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="151">
@@ -5732,7 +5732,7 @@
         <v>0</v>
       </c>
       <c r="K151" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="152">
@@ -5767,7 +5767,7 @@
         <v>0</v>
       </c>
       <c r="K152" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153">
@@ -5802,7 +5802,7 @@
         <v>1</v>
       </c>
       <c r="K153" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="154">
@@ -5942,7 +5942,7 @@
         <v>1</v>
       </c>
       <c r="K157" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="158">
@@ -6012,7 +6012,7 @@
         <v>1</v>
       </c>
       <c r="K159" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="160">
@@ -6222,7 +6222,7 @@
         <v>0</v>
       </c>
       <c r="K165" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="166">
@@ -6257,7 +6257,7 @@
         <v>0</v>
       </c>
       <c r="K166" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="167">
@@ -6292,7 +6292,7 @@
         <v>0</v>
       </c>
       <c r="K167" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="168">
@@ -6327,7 +6327,7 @@
         <v>1</v>
       </c>
       <c r="K168" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="169">
@@ -6467,7 +6467,7 @@
         <v>1</v>
       </c>
       <c r="K172" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="173">
@@ -6537,7 +6537,7 @@
         <v>1</v>
       </c>
       <c r="K174" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="175">
@@ -6747,7 +6747,7 @@
         <v>0</v>
       </c>
       <c r="K180" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="181">
@@ -6782,7 +6782,7 @@
         <v>0</v>
       </c>
       <c r="K181" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="182">
@@ -6817,7 +6817,7 @@
         <v>0</v>
       </c>
       <c r="K182" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="183">
@@ -6852,7 +6852,7 @@
         <v>1</v>
       </c>
       <c r="K183" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="184">
@@ -6992,7 +6992,7 @@
         <v>1</v>
       </c>
       <c r="K187" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="188">
@@ -7062,7 +7062,7 @@
         <v>1</v>
       </c>
       <c r="K189" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="190">
@@ -7272,7 +7272,7 @@
         <v>0</v>
       </c>
       <c r="K195" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="196">
@@ -7307,7 +7307,7 @@
         <v>0</v>
       </c>
       <c r="K196" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="197">
@@ -7342,7 +7342,7 @@
         <v>0</v>
       </c>
       <c r="K197" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="198">
@@ -7377,7 +7377,7 @@
         <v>1</v>
       </c>
       <c r="K198" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="199">
@@ -7517,7 +7517,7 @@
         <v>1</v>
       </c>
       <c r="K202" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="203">
@@ -7587,7 +7587,7 @@
         <v>1</v>
       </c>
       <c r="K204" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="205">
@@ -7797,7 +7797,7 @@
         <v>0</v>
       </c>
       <c r="K210" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="211">
@@ -7832,7 +7832,7 @@
         <v>0</v>
       </c>
       <c r="K211" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="212">
@@ -7867,7 +7867,7 @@
         <v>0</v>
       </c>
       <c r="K212" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="213">
@@ -7902,7 +7902,7 @@
         <v>1</v>
       </c>
       <c r="K213" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="214">
@@ -8042,7 +8042,7 @@
         <v>1</v>
       </c>
       <c r="K217" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="218">
@@ -8112,7 +8112,7 @@
         <v>1</v>
       </c>
       <c r="K219" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="220">
@@ -8322,7 +8322,7 @@
         <v>0</v>
       </c>
       <c r="K225" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="226">
@@ -8357,7 +8357,7 @@
         <v>0</v>
       </c>
       <c r="K226" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="227">
@@ -8392,7 +8392,7 @@
         <v>0</v>
       </c>
       <c r="K227" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="228">
@@ -8427,7 +8427,7 @@
         <v>1</v>
       </c>
       <c r="K228" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="229">
@@ -8567,7 +8567,7 @@
         <v>1</v>
       </c>
       <c r="K232" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="233">
@@ -8637,7 +8637,7 @@
         <v>1</v>
       </c>
       <c r="K234" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="235">
@@ -8847,7 +8847,7 @@
         <v>0</v>
       </c>
       <c r="K240" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="241">
@@ -8882,7 +8882,7 @@
         <v>0</v>
       </c>
       <c r="K241" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="242">
@@ -8917,7 +8917,7 @@
         <v>0</v>
       </c>
       <c r="K242" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="243">
@@ -8952,7 +8952,7 @@
         <v>1</v>
       </c>
       <c r="K243" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="244">
@@ -9092,7 +9092,7 @@
         <v>1</v>
       </c>
       <c r="K247" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="248">
@@ -9162,7 +9162,7 @@
         <v>1</v>
       </c>
       <c r="K249" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="250">
@@ -9372,7 +9372,7 @@
         <v>0</v>
       </c>
       <c r="K255" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="256">
@@ -9407,7 +9407,7 @@
         <v>0</v>
       </c>
       <c r="K256" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="257">
@@ -9442,7 +9442,7 @@
         <v>0</v>
       </c>
       <c r="K257" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="258">
@@ -9477,7 +9477,7 @@
         <v>1</v>
       </c>
       <c r="K258" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="259">
@@ -9617,7 +9617,7 @@
         <v>1</v>
       </c>
       <c r="K262" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="263">
@@ -9687,7 +9687,7 @@
         <v>1</v>
       </c>
       <c r="K264" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="265">
@@ -9897,7 +9897,7 @@
         <v>0</v>
       </c>
       <c r="K270" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="271">
@@ -9932,7 +9932,42 @@
         <v>0</v>
       </c>
       <c r="K271" t="n">
-        <v>2</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" s="1" t="n">
+        <v>270</v>
+      </c>
+      <c r="B272" t="n">
+        <v>10000</v>
+      </c>
+      <c r="C272" t="n">
+        <v>3</v>
+      </c>
+      <c r="D272" t="n">
+        <v>2</v>
+      </c>
+      <c r="E272" t="n">
+        <v>12</v>
+      </c>
+      <c r="F272" t="n">
+        <v>1</v>
+      </c>
+      <c r="G272" t="n">
+        <v>1</v>
+      </c>
+      <c r="H272" t="n">
+        <v>0</v>
+      </c>
+      <c r="I272" t="n">
+        <v>1</v>
+      </c>
+      <c r="J272" t="n">
+        <v>0</v>
+      </c>
+      <c r="K272" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>